<commit_message>
sn 5 rating curve
</commit_message>
<xml_diff>
--- a/Discharge/RatingCurves/Stn5.xlsx
+++ b/Discharge/RatingCurves/Stn5.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/kriddie_ad_unc_edu/Documents/Ecuador2021/Ecuador2021/Discharge/RatingCurves/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/LongTermData_CayambeCoca/Discharge/RatingCurves/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{D2AA75E7-7C39-4662-8711-B7604104F4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E276AE8E-5B9C-AA4E-A3C7-28F4B7A15F35}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A81247-45FF-4E45-8871-76E602A17C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6380" yWindow="3000" windowWidth="25480" windowHeight="13820" xr2:uid="{515098AF-24E6-42D4-AB1F-FD9DF5411C44}"/>
+    <workbookView xWindow="780" yWindow="1600" windowWidth="26720" windowHeight="17580" xr2:uid="{515098AF-24E6-42D4-AB1F-FD9DF5411C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$D$20:$D$25</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$E$20:$E$25</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -62,12 +66,15 @@
   <si>
     <t>missing Baro data - average July 27 14:45  July 28 14:15   (0.5582355+0.5118179)/2</t>
   </si>
+  <si>
+    <t>Station 5 2 parts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,20 +84,27 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
       <family val="2"/>
@@ -116,15 +130,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +600,864 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11657655293088363"/>
+                  <c:y val="-8.3750000000000005E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$20:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.2337899999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91951210000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73393330000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57524439999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56698470000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55664480000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53502669999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4680107</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55452369999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4703968</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.44459789999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$20:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.1282000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78110000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21695999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16736999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13866000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10291500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.1770999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4549999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.018999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.0860000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.7079999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EB32-0B4C-A226-9FC26174DD2D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="379811567"/>
+        <c:axId val="401111519"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="379811567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="401111519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="401111519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="379811567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.34217716535433068"/>
+                  <c:y val="-0.14413385826771655"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$25:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.55664480000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53502669999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4680107</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55452369999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4703968</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44459789999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$25:$E$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.10291500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1770999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4549999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.018999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0860000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.7079999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DFC4-5B47-85E5-7DE7FDA9A71A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="246831295"/>
+        <c:axId val="246875263"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="246831295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="246875263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="246875263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="246831295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1141,20 +2013,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>250825</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>22225</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>253999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>555625</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>365124</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>282574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1174,6 +3078,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{681E30BE-9336-6BCB-4CB7-B0F08EB0EA01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>311150</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F968DA2-2FCE-3CC2-11CB-ED1E7A80393A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1479,237 +3455,502 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF96F4BF-E92E-4DEB-9357-8C809523DCE6}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>44358</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>0.53333333333333333</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>0.53125</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>0.44459789999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>4.7079999999999997E-2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>44386</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>0.67361111111111116</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>0.67708333333333337</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>0.57524439999999999</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.16736999999999999</v>
       </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>44391</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>0.60902777777777783</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>0.4703968</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>5.0860000000000002E-2</v>
       </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>44393</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>0.58819444444444446</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>0.4680107</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>6.4549999999999996E-2</v>
       </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>44398</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="4">
         <v>0.45</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>0.73393330000000001</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.21695999999999999</v>
       </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>44400</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="4">
         <v>0.41319444444444442</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>0.91951210000000005</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.78110000000000002</v>
       </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>44403</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="4">
         <v>0.61458333333333337</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>0.61458333333333337</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>0.56698470000000001</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>0.13866000000000001</v>
       </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>44405</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="4">
         <v>0.5625</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>0.5625</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <f>(0.5582355+0.5118179)/2</f>
         <v>0.53502669999999997</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>8.1770999999999996E-2</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>44396</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="4">
         <v>0.4236111111111111</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <v>1.2337899999999999</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>1.1282000000000001</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="G11" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="12" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>44740</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="4">
         <v>0.55138888888888882</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <v>0.5625</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>0.55664480000000005</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>0.10291500000000001</v>
       </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
         <v>44768</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="4">
         <v>0.43611111111111112</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>0.4375</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>0.55452369999999995</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>6.018999999999998E-2</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="18" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>44396</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1.2337899999999999</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.1282000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>44400</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.91951210000000005</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.78110000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>44398</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.73393330000000001</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.21695999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>44386</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.57524439999999999</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.16736999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>44403</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.56698470000000001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.13866000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>44740</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.55138888888888882</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="D25" s="6">
+        <v>0.55664480000000005</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.10291500000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>44405</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.5625</v>
+      </c>
+      <c r="D26" s="2">
+        <f>(0.5582355+0.5118179)/2</f>
+        <v>0.53502669999999997</v>
+      </c>
+      <c r="E26" s="2">
+        <v>8.1770999999999996E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>44393</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0.4680107</v>
+      </c>
+      <c r="E27" s="2">
+        <v>6.4549999999999996E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>44768</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.4375</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.55452369999999995</v>
+      </c>
+      <c r="E28" s="2">
+        <v>6.018999999999998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>44391</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.60902777777777783</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.4703968</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5.0860000000000002E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>44358</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.53125</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.44459789999999999</v>
+      </c>
+      <c r="E30" s="2">
+        <v>4.7079999999999997E-2</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A20:E30">
+    <sortCondition descending="1" ref="E20:E30"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>